<commit_message>
modified:   client/public/fichiers/ANNEXE 19 - TABLEAU DE DETERMINATION DU PRIX DE VENTE DES PRODUITS.xlsx
</commit_message>
<xml_diff>
--- a/client/public/fichiers/ANNEXE 19 - TABLEAU DE DETERMINATION DU PRIX DE VENTE DES PRODUITS.xlsx
+++ b/client/public/fichiers/ANNEXE 19 - TABLEAU DE DETERMINATION DU PRIX DE VENTE DES PRODUITS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://219295cocerto-my.sharepoint.com/personal/lgombaud_cocerto_fr/Documents/SAUVEGARDE LOCAL LG/MEMOIRE DEC/MEMOIRE/ANNEXE/ANNEXE 19 - TABLEAU DE DETERMINATION DU PRIX DE VENTE DES PRODUITS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgombaud\Documents\DEF MEMOIRE\ANNEXES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{6EF831EE-EF2C-4FC5-B09A-77E59F155C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A5D2033-A12A-4A18-98A3-6602474A8450}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEE2417-F28D-42DD-A75A-8D03ADE70B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{7AF6AC51-9839-4727-8932-D1008C440D98}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7AF6AC51-9839-4727-8932-D1008C440D98}"/>
   </bookViews>
   <sheets>
     <sheet name="📘 Notice" sheetId="4" r:id="rId1"/>
@@ -797,7 +797,7 @@
     </r>
   </si>
   <si>
-    <t>Informations du projet</t>
+    <t>INFORMATIONS DU PROJET</t>
   </si>
   <si>
     <t>Élément</t>
@@ -866,7 +866,7 @@
     <t>À compléter, ex: 20%,10%,5,5% ou 0 si exonération</t>
   </si>
   <si>
-    <t>Coût de revient projet</t>
+    <t>COUT DE REVIENT PROJET</t>
   </si>
   <si>
     <t>Catégorie de coût</t>
@@ -893,6 +893,48 @@
     <t>A. Matières premières &amp; Consommables</t>
   </si>
   <si>
+    <t>Matière première 1 (ex. : Acier, bois, etc.)</t>
+  </si>
+  <si>
+    <t>[kg, m, ml,  pièce, L, pot]</t>
+  </si>
+  <si>
+    <t>Facture n°[] - [Date] - [Fournisseur]</t>
+  </si>
+  <si>
+    <t>Matière première 2 (ex. : Acier, bois, etc.)</t>
+  </si>
+  <si>
+    <t>Matière première 3 (ex. : Acier, bois, etc.)</t>
+  </si>
+  <si>
+    <t>Matière première 4 (ex. : Acier, bois, etc.)</t>
+  </si>
+  <si>
+    <t>Consommables 1 (ex. : visserie, colle, abrasifs, peinture, etc.)</t>
+  </si>
+  <si>
+    <t>Consommables 2 (ex. : visserie, colle, abrasifs, peinture, etc.)</t>
+  </si>
+  <si>
+    <t>Consommables 3 (ex. : visserie, colle, abrasifs, peinture, etc.)</t>
+  </si>
+  <si>
+    <t>Consommables 4 (ex. : visserie, colle, abrasifs, peinture, etc.)</t>
+  </si>
+  <si>
+    <t>Fourniture spécifique 1 (ex. : acheté spécifiquement pour la fabrication)</t>
+  </si>
+  <si>
+    <t>Fourniture spécifique 2 (ex. : acheté spécifiquement pour la fabrication)</t>
+  </si>
+  <si>
+    <t>Fourniture spécifique 3 (ex. : acheté spécifiquement pour la fabrication)</t>
+  </si>
+  <si>
+    <t>Fourniture spécifique 4 (ex. : acheté spécifiquement pour la fabrication)</t>
+  </si>
+  <si>
     <t>Total A - Coût matières directes</t>
   </si>
   <si>
@@ -941,7 +983,7 @@
     <t>TOTAL COÛTS PROJET (A+B+C)</t>
   </si>
   <si>
-    <t>Prix de vente</t>
+    <t>PRIX DE VENTE</t>
   </si>
   <si>
     <t>Montant (€)</t>
@@ -953,6 +995,9 @@
     <t>Prix de vente d'une unité, à fixer en fonction du marché</t>
   </si>
   <si>
+    <t>Taux de TVA applicable</t>
+  </si>
+  <si>
     <t>Coût de revient unitaire (hors temps élèves)</t>
   </si>
   <si>
@@ -1073,9 +1118,15 @@
     <t>Marge nette (%) théorique</t>
   </si>
   <si>
+    <t>Marge nette théorique / Prix de vente hors taxes</t>
+  </si>
+  <si>
     <t>Marge nette (%) réelle</t>
   </si>
   <si>
+    <t>Marge nette réelle / Prix de vente hors taxes</t>
+  </si>
+  <si>
     <t>Contrôle marge nette projet</t>
   </si>
   <si>
@@ -1095,57 +1146,6 @@
   </si>
   <si>
     <t xml:space="preserve">Marge nette du projet réelle - Marge nette du projet théorique </t>
-  </si>
-  <si>
-    <t>Taux de TVA applicable</t>
-  </si>
-  <si>
-    <t>Marge nette théorique / Prix de vente hors taxes</t>
-  </si>
-  <si>
-    <t>Marge nette réelle / Prix de vente hors taxes</t>
-  </si>
-  <si>
-    <t>Matière première 1 (ex. : Acier, bois, etc.)</t>
-  </si>
-  <si>
-    <t>Matière première 2 (ex. : Acier, bois, etc.)</t>
-  </si>
-  <si>
-    <t>Matière première 3 (ex. : Acier, bois, etc.)</t>
-  </si>
-  <si>
-    <t>Matière première 4 (ex. : Acier, bois, etc.)</t>
-  </si>
-  <si>
-    <t>Consommables 1 (ex. : visserie, colle, abrasifs, peinture, etc.)</t>
-  </si>
-  <si>
-    <t>Consommables 2 (ex. : visserie, colle, abrasifs, peinture, etc.)</t>
-  </si>
-  <si>
-    <t>Consommables 3 (ex. : visserie, colle, abrasifs, peinture, etc.)</t>
-  </si>
-  <si>
-    <t>Consommables 4 (ex. : visserie, colle, abrasifs, peinture, etc.)</t>
-  </si>
-  <si>
-    <t>Fourniture spécifique 1 (ex. : acheté spécifiquement pour la fabrication)</t>
-  </si>
-  <si>
-    <t>Fourniture spécifique 2 (ex. : acheté spécifiquement pour la fabrication)</t>
-  </si>
-  <si>
-    <t>Fourniture spécifique 3 (ex. : acheté spécifiquement pour la fabrication)</t>
-  </si>
-  <si>
-    <t>Fourniture spécifique 4 (ex. : acheté spécifiquement pour la fabrication)</t>
-  </si>
-  <si>
-    <t>[kg, m, ml,  pièce, L, pot]</t>
-  </si>
-  <si>
-    <t>Facture n°[] - [Date] - [Fournisseur]</t>
   </si>
 </sst>
 </file>
@@ -1156,7 +1156,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-40C]_-;\-* #,##0.00\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1285,52 +1285,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF555555"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF555555"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -1418,7 +1372,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1583,12 +1537,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1712,9 +1711,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -1785,49 +1781,33 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="10" fontId="6" fillId="14" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="22" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1854,9 +1834,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="14" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2373,7 +2350,7 @@
   </sheetPr>
   <dimension ref="A1:A82"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2434,7 +2411,7 @@
       </c>
     </row>
     <row r="17" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="59" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2450,7 +2427,7 @@
       <c r="A20" s="16"/>
     </row>
     <row r="21" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="60" t="s">
+      <c r="A21" s="59" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2503,7 +2480,7 @@
       <c r="A35" s="16"/>
     </row>
     <row r="36" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="63" t="s">
+      <c r="A36" s="62" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2639,7 +2616,7 @@
       <c r="A70" s="21"/>
     </row>
     <row r="71" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="77" t="s">
+      <c r="A71" s="62" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2658,7 +2635,7 @@
       <c r="A75" s="21"/>
     </row>
     <row r="76" spans="1:1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A76" s="78" t="s">
+      <c r="A76" s="60" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2666,7 +2643,7 @@
       <c r="A77" s="22"/>
     </row>
     <row r="78" spans="1:1" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A78" s="61" t="s">
+      <c r="A78" s="60" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2682,7 +2659,7 @@
       <c r="A81" s="23"/>
     </row>
     <row r="82" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="61" t="s">
+      <c r="A82" s="60" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2728,11 +2705,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -2761,7 +2738,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>44</v>
@@ -2777,7 +2754,7 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:11" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>45</v>
@@ -2787,7 +2764,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:11" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>47</v>
@@ -2797,7 +2774,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:11" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>48</v>
@@ -2807,7 +2784,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:11" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>49</v>
@@ -2817,7 +2794,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
@@ -2827,7 +2804,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:11" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
@@ -2837,7 +2814,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:12" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:12" s="3" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>54</v>
@@ -2854,7 +2831,7 @@
       <c r="K18" s="6"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:12" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:12" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>55</v>
@@ -2864,7 +2841,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="31"/>
     </row>
     <row r="22" spans="1:12" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2876,7 +2853,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="31"/>
     </row>
     <row r="24" spans="1:12" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2888,7 +2865,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="31"/>
     </row>
     <row r="26" spans="1:12" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2936,14 +2913,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -2975,7 +2952,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -2989,14 +2966,14 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="82"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="76"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -3004,14 +2981,14 @@
       <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:11" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="84" t="s">
+      <c r="A5" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -3019,20 +2996,20 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="52" t="s">
-        <v>143</v>
-      </c>
-      <c r="B6" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="49">
+      <c r="A6" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="47"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="48">
         <f>C6*D6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="59" t="s">
-        <v>156</v>
+      <c r="F6" s="58" t="s">
+        <v>74</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -3041,20 +3018,20 @@
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="52" t="s">
-        <v>144</v>
-      </c>
-      <c r="B7" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="49">
+      <c r="A7" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="47"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="48">
         <f t="shared" ref="E7:E17" si="0">C7*D7</f>
         <v>0</v>
       </c>
-      <c r="F7" s="59" t="s">
-        <v>156</v>
+      <c r="F7" s="58" t="s">
+        <v>74</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -3063,20 +3040,20 @@
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="52" t="s">
-        <v>145</v>
-      </c>
-      <c r="B8" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="49">
+      <c r="A8" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="47"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F8" s="59" t="s">
-        <v>156</v>
+      <c r="F8" s="58" t="s">
+        <v>74</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -3085,20 +3062,20 @@
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="52" t="s">
-        <v>146</v>
-      </c>
-      <c r="B9" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="49">
+      <c r="A9" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="47"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F9" s="59" t="s">
-        <v>156</v>
+      <c r="F9" s="58" t="s">
+        <v>74</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -3107,20 +3084,20 @@
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
-        <v>147</v>
-      </c>
-      <c r="B10" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="49">
+      <c r="A10" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="47"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F10" s="59" t="s">
-        <v>156</v>
+      <c r="F10" s="58" t="s">
+        <v>74</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -3129,20 +3106,20 @@
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52" t="s">
-        <v>148</v>
-      </c>
-      <c r="B11" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="49">
+      <c r="A11" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="47"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F11" s="59" t="s">
-        <v>156</v>
+      <c r="F11" s="58" t="s">
+        <v>74</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -3151,20 +3128,20 @@
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="52" t="s">
-        <v>149</v>
-      </c>
-      <c r="B12" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="49">
+      <c r="A12" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="47"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="48">
         <f>C12*D12</f>
         <v>0</v>
       </c>
-      <c r="F12" s="59" t="s">
-        <v>156</v>
+      <c r="F12" s="58" t="s">
+        <v>74</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -3173,20 +3150,20 @@
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="52" t="s">
-        <v>150</v>
-      </c>
-      <c r="B13" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="49">
+      <c r="A13" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="47"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="48">
         <f>C13*D13</f>
         <v>0</v>
       </c>
-      <c r="F13" s="59" t="s">
-        <v>156</v>
+      <c r="F13" s="58" t="s">
+        <v>74</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -3195,20 +3172,20 @@
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="52" t="s">
-        <v>151</v>
-      </c>
-      <c r="B14" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="C14" s="48"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="49">
+      <c r="A14" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="47"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F14" s="59" t="s">
-        <v>156</v>
+      <c r="F14" s="58" t="s">
+        <v>74</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -3217,20 +3194,20 @@
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B15" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="49">
+      <c r="A15" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="47"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F15" s="59" t="s">
-        <v>156</v>
+      <c r="F15" s="58" t="s">
+        <v>74</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -3239,20 +3216,20 @@
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52" t="s">
-        <v>153</v>
-      </c>
-      <c r="B16" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="49">
+      <c r="A16" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="47"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F16" s="59" t="s">
-        <v>156</v>
+      <c r="F16" s="58" t="s">
+        <v>74</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -3261,25 +3238,25 @@
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:6" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="52" t="s">
-        <v>154</v>
-      </c>
-      <c r="B17" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="49">
+      <c r="A17" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="47"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F17" s="59" t="s">
-        <v>156</v>
+      <c r="F17" s="58" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -3290,7 +3267,7 @@
       </c>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -3299,69 +3276,69 @@
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="85" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" s="85"/>
-      <c r="C20" s="85"/>
-      <c r="D20" s="85"/>
-      <c r="E20" s="85"/>
-      <c r="F20" s="85"/>
+      <c r="A20" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="79"/>
+      <c r="C20" s="79"/>
+      <c r="D20" s="79"/>
+      <c r="E20" s="79"/>
+      <c r="F20" s="79"/>
     </row>
     <row r="21" spans="1:6" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="53" t="s">
+      <c r="A21" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="47"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="48">
+        <f>C21*D21</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="51" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="49">
-        <f>C21*D21</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="59" t="s">
-        <v>156</v>
-      </c>
     </row>
     <row r="22" spans="1:6" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="53" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="51" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="48"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="49">
+      <c r="A22" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="47"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="48">
         <f t="shared" ref="E22:E23" si="1">C22*D22</f>
         <v>0</v>
       </c>
-      <c r="F22" s="59" t="s">
-        <v>156</v>
+      <c r="F22" s="58" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="53" t="s">
-        <v>77</v>
-      </c>
-      <c r="B23" s="51" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="49">
+      <c r="A23" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="47"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F23" s="59" t="s">
-        <v>156</v>
+      <c r="F23" s="58" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -3372,7 +3349,7 @@
       </c>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" s="4" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -3381,19 +3358,19 @@
       <c r="F25" s="6"/>
     </row>
     <row r="26" spans="1:6" s="4" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="54" t="s">
-        <v>79</v>
+      <c r="A26" s="53" t="s">
+        <v>93</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
-      <c r="E26" s="50">
+      <c r="E26" s="49">
         <f>E18+E24</f>
         <v>0</v>
       </c>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -3402,41 +3379,41 @@
       <c r="F27" s="6"/>
     </row>
     <row r="28" spans="1:6" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="85" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" s="85"/>
-      <c r="C28" s="85"/>
-      <c r="D28" s="85"/>
-      <c r="E28" s="85"/>
-      <c r="F28" s="85"/>
+      <c r="A28" s="79" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="79"/>
+      <c r="C28" s="79"/>
+      <c r="D28" s="79"/>
+      <c r="E28" s="79"/>
+      <c r="F28" s="79"/>
     </row>
     <row r="29" spans="1:6" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="53" t="s">
-        <v>81</v>
-      </c>
-      <c r="B29" s="51" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="57">
+      <c r="A29" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="56">
         <f>'🧮 Fiche produit'!B20</f>
         <v>0</v>
       </c>
-      <c r="D29" s="49">
+      <c r="D29" s="48">
         <f>'🧮 Fiche produit'!B22</f>
         <v>0</v>
       </c>
-      <c r="E29" s="49">
+      <c r="E29" s="48">
         <f>C29*D29</f>
         <v>0</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -3447,7 +3424,7 @@
       </c>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" s="4" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -3456,19 +3433,19 @@
       <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:6" s="4" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="54" t="s">
-        <v>85</v>
+      <c r="A32" s="53" t="s">
+        <v>99</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="50">
+      <c r="E32" s="49">
         <f>E24+E30+E18</f>
         <v>0</v>
       </c>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -3482,30 +3459,31 @@
       <c r="K33" s="1"/>
     </row>
     <row r="34" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="80" t="s">
-        <v>86</v>
-      </c>
-      <c r="B34" s="81"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="81"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="82"/>
+      <c r="A34" s="74" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" s="75"/>
+      <c r="C34" s="75"/>
+      <c r="D34" s="75"/>
+      <c r="E34" s="75"/>
+      <c r="F34" s="76"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
     </row>
+    <row r="35" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="B36" s="6"/>
-      <c r="C36" s="57">
+      <c r="C36" s="56">
         <f>'🧮 Fiche produit'!$B$24</f>
         <v>0</v>
       </c>
-      <c r="D36" s="49">
+      <c r="D36" s="48">
         <f>E18</f>
         <v>0</v>
       </c>
@@ -3522,14 +3500,14 @@
     </row>
     <row r="37" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="B37" s="6"/>
-      <c r="C37" s="57">
+      <c r="C37" s="56">
         <f>'🧮 Fiche produit'!$B$24</f>
         <v>0</v>
       </c>
-      <c r="D37" s="49">
+      <c r="D37" s="48">
         <f>E24</f>
         <v>0</v>
       </c>
@@ -3544,14 +3522,15 @@
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
     </row>
+    <row r="38" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="54" t="s">
-        <v>79</v>
+      <c r="A39" s="53" t="s">
+        <v>93</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
-      <c r="E39" s="50">
+      <c r="E39" s="49">
         <f>E36+E37</f>
         <v>0</v>
       </c>
@@ -3562,16 +3541,17 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
+    <row r="40" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="B41" s="6"/>
-      <c r="C41" s="57">
+      <c r="C41" s="56">
         <f>'🧮 Fiche produit'!$B$24</f>
         <v>0</v>
       </c>
-      <c r="D41" s="49">
+      <c r="D41" s="48">
         <f>E30</f>
         <v>0</v>
       </c>
@@ -3586,14 +3566,15 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
+    <row r="42" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="54" t="s">
-        <v>87</v>
+      <c r="A43" s="53" t="s">
+        <v>101</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
-      <c r="E43" s="50">
+      <c r="E43" s="49">
         <f>E39+E41</f>
         <v>0</v>
       </c>
@@ -3639,9 +3620,9 @@
   </sheetPr>
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3653,16 +3634,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="86" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
+      <c r="A1" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12"/>
       <c r="B2" s="12" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>43</v>
@@ -3678,139 +3659,139 @@
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" s="42"/>
+        <v>104</v>
+      </c>
+      <c r="B3" s="41"/>
       <c r="C3" s="8" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="88">
+      <c r="B4" s="63">
         <f>'🧮 Fiche produit'!B26</f>
         <v>0</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="43">
+        <v>107</v>
+      </c>
+      <c r="B6" s="42">
         <f>'🧱 Coût de revient'!$E$26</f>
         <v>0</v>
       </c>
-      <c r="C6" s="44" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="43" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B8" s="43">
+        <v>109</v>
+      </c>
+      <c r="B8" s="42">
         <f>B3-B6</f>
         <v>0</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" s="43">
+        <v>111</v>
+      </c>
+      <c r="B9" s="42">
         <f>B8*'🧮 Fiche produit'!B24</f>
         <v>0</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="B10" s="56" t="str">
+      <c r="A10" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="55" t="str">
         <f>IF(B3="","",B8/B3)</f>
         <v/>
       </c>
-      <c r="C10" s="46" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="45" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="2" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:11" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="40" t="s">
-        <v>100</v>
-      </c>
-      <c r="B12" s="41">
+        <v>115</v>
+      </c>
+      <c r="B12" s="69">
         <f>'🧱 Coût de revient'!E32</f>
         <v>0</v>
       </c>
-      <c r="C12" s="44" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="68" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="B14" s="47">
+        <v>117</v>
+      </c>
+      <c r="B14" s="46">
         <f>B3-B12</f>
         <v>0</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B15" s="47">
+        <v>119</v>
+      </c>
+      <c r="B15" s="46">
         <f>B14*'🧮 Fiche produit'!B24</f>
         <v>0</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
-        <v>106</v>
-      </c>
-      <c r="B16" s="56" t="str">
+      <c r="A16" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" s="55" t="str">
         <f>IF(B3="","",B14/B3)</f>
         <v/>
       </c>
-      <c r="C16" s="46" t="s">
-        <v>107</v>
+      <c r="C16" s="45" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3819,100 +3800,100 @@
       <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:11" s="2" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="87" t="s">
-        <v>108</v>
-      </c>
-      <c r="B18" s="87"/>
-      <c r="C18" s="87"/>
-    </row>
-    <row r="19" spans="1:11" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A18" s="81" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="81"/>
+      <c r="C18" s="81"/>
+    </row>
+    <row r="19" spans="1:11" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:11" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="B20" s="39">
         <f>'🧱 Coût de revient'!E32</f>
         <v>0</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
     </row>
     <row r="22" spans="1:11" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="B22" s="55"/>
+        <v>126</v>
+      </c>
+      <c r="B22" s="54"/>
       <c r="C22" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:11" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="s">
-        <v>113</v>
-      </c>
-      <c r="B24" s="41">
+        <v>128</v>
+      </c>
+      <c r="B24" s="71">
         <f>(B20)/(1-B22)</f>
         <v>0</v>
       </c>
-      <c r="C24" s="8"/>
+      <c r="C24" s="70"/>
     </row>
     <row r="25" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="B25" s="41">
+        <v>129</v>
+      </c>
+      <c r="B25" s="72">
         <f>B24*'🧮 Fiche produit'!B24</f>
         <v>0</v>
       </c>
-      <c r="C25" s="8"/>
-    </row>
-    <row r="26" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="70"/>
+    </row>
+    <row r="26" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="40" t="s">
-        <v>115</v>
-      </c>
-      <c r="B27" s="41">
+        <v>130</v>
+      </c>
+      <c r="B27" s="71">
         <f>B24*(1+B4)</f>
         <v>0</v>
       </c>
-      <c r="C27" s="8"/>
+      <c r="C27" s="70"/>
     </row>
     <row r="28" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="40" t="s">
-        <v>116</v>
-      </c>
-      <c r="B28" s="41">
+        <v>131</v>
+      </c>
+      <c r="B28" s="72">
         <f>B27*'🧮 Fiche produit'!B24</f>
         <v>0</v>
       </c>
-      <c r="C28" s="8"/>
+      <c r="C28" s="70"/>
     </row>
     <row r="29" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="62"/>
-      <c r="B29" s="62"/>
-      <c r="C29" s="62"/>
+      <c r="A29" s="61"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="61"/>
     </row>
     <row r="30" spans="1:11" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="B30" s="87"/>
-      <c r="C30" s="87"/>
+      <c r="A30" s="81" t="s">
+        <v>132</v>
+      </c>
+      <c r="B30" s="81"/>
+      <c r="C30" s="81"/>
     </row>
     <row r="31" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
@@ -3920,12 +3901,12 @@
       <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="64" t="s">
-        <v>118</v>
-      </c>
-      <c r="B32" s="65"/>
+      <c r="A32" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B32" s="30"/>
       <c r="C32" s="8" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -3936,7 +3917,7 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -3951,14 +3932,14 @@
     </row>
     <row r="34" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="B34" s="43">
+        <v>135</v>
+      </c>
+      <c r="B34" s="42">
         <f>'🧱 Coût de revient'!E30</f>
         <v>0</v>
       </c>
-      <c r="C34" s="44" t="s">
-        <v>121</v>
+      <c r="C34" s="43" t="s">
+        <v>136</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -3970,15 +3951,15 @@
       <c r="K34" s="2"/>
     </row>
     <row r="35" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="69" t="s">
-        <v>122</v>
-      </c>
-      <c r="B35" s="66">
+      <c r="A35" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B35" s="42">
         <f>B32*'🧮 Fiche produit'!B22</f>
         <v>0</v>
       </c>
-      <c r="C35" s="67" t="s">
-        <v>123</v>
+      <c r="C35" s="43" t="s">
+        <v>138</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -3989,10 +3970,10 @@
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="68"/>
-      <c r="B36" s="68"/>
-      <c r="C36" s="68"/>
+    <row r="36" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -4003,11 +3984,11 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="73" t="s">
-        <v>124</v>
-      </c>
-      <c r="B37" s="73"/>
-      <c r="C37" s="73"/>
+      <c r="A37" s="64" t="s">
+        <v>139</v>
+      </c>
+      <c r="B37" s="64"/>
+      <c r="C37" s="64"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -4017,10 +3998,10 @@
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="68"/>
-      <c r="B38" s="68"/>
-      <c r="C38" s="68"/>
+    <row r="38" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
@@ -4032,14 +4013,14 @@
     </row>
     <row r="39" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B39" s="43">
+        <v>140</v>
+      </c>
+      <c r="B39" s="42">
         <f>B3-B6-B34</f>
         <v>0</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -4052,14 +4033,14 @@
     </row>
     <row r="40" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="B40" s="43">
+        <v>142</v>
+      </c>
+      <c r="B40" s="42">
         <f>B3-B6-B35</f>
         <v>0</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -4072,14 +4053,14 @@
     </row>
     <row r="41" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B41" s="43">
+        <v>144</v>
+      </c>
+      <c r="B41" s="42">
         <f>B40-B39</f>
         <v>0</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -4091,15 +4072,15 @@
       <c r="K41" s="2"/>
     </row>
     <row r="42" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="45" t="s">
-        <v>131</v>
-      </c>
-      <c r="B42" s="56" t="str">
+      <c r="A42" s="44" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" s="55" t="str">
         <f>IF(B3="","",B39/B3)</f>
         <v/>
       </c>
-      <c r="C42" s="46" t="s">
-        <v>141</v>
+      <c r="C42" s="45" t="s">
+        <v>147</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -4111,15 +4092,15 @@
       <c r="K42" s="2"/>
     </row>
     <row r="43" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="71" t="s">
-        <v>132</v>
-      </c>
-      <c r="B43" s="72" t="str">
+      <c r="A43" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B43" s="55" t="str">
         <f>IF(B3="","",B40/B3)</f>
         <v/>
       </c>
-      <c r="C43" s="46" t="s">
-        <v>142</v>
+      <c r="C43" s="45" t="s">
+        <v>149</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -4130,10 +4111,10 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="74"/>
-      <c r="B44" s="75"/>
-      <c r="C44" s="76"/>
+    <row r="44" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="65"/>
+      <c r="B44" s="66"/>
+      <c r="C44" s="67"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
@@ -4144,11 +4125,11 @@
       <c r="K44" s="2"/>
     </row>
     <row r="45" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="73" t="s">
-        <v>133</v>
-      </c>
-      <c r="B45" s="73"/>
-      <c r="C45" s="73"/>
+      <c r="A45" s="64" t="s">
+        <v>150</v>
+      </c>
+      <c r="B45" s="64"/>
+      <c r="C45" s="64"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
@@ -4158,10 +4139,10 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="68"/>
-      <c r="B46" s="68"/>
-      <c r="C46" s="68"/>
+    <row r="46" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
@@ -4173,38 +4154,38 @@
     </row>
     <row r="47" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B47" s="47">
+        <v>151</v>
+      </c>
+      <c r="B47" s="46">
         <f>'🧮 Fiche produit'!B24*B39</f>
         <v>0</v>
       </c>
-      <c r="C47" s="70" t="s">
-        <v>135</v>
+      <c r="C47" s="8" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="B48" s="47">
+        <v>153</v>
+      </c>
+      <c r="B48" s="46">
         <f>'🧮 Fiche produit'!B24*B40</f>
         <v>0</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="69" t="s">
-        <v>138</v>
-      </c>
-      <c r="B49" s="66">
+      <c r="A49" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B49" s="42">
         <f>B48-B47</f>
         <v>0</v>
       </c>
-      <c r="C49" s="70" t="s">
-        <v>139</v>
+      <c r="C49" s="8" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>